<commit_message>
Módulo 11 - Fórmulas avançadas (PGTO-VF-VP)
</commit_message>
<xml_diff>
--- a/Módulo 11 - Formulas avançadas/aula-financeiras.xlsx
+++ b/Módulo 11 - Formulas avançadas/aula-financeiras.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelio\Google Drive\Cursos online\Curso_Excel\10 Fórmulas avançadas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\Módulo 11 - Formulas avançadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6780"/>
   </bookViews>
   <sheets>
     <sheet name="Financeiras" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>EducandoWeb</t>
   </si>
@@ -113,15 +113,35 @@
   <si>
     <t>Valor financiado ($)</t>
   </si>
+  <si>
+    <t>=PGTO(C10;C9;-C8;0;0)</t>
+  </si>
+  <si>
+    <t>valor presente é o valor a ser financiado</t>
+  </si>
+  <si>
+    <t>=PGTO(taxa de juros;numero de periodos;Valor presente;
+valor futuro;quando o pagamento irá acontecer)</t>
+  </si>
+  <si>
+    <t>=VP(F10;F9;0;-F6;0)</t>
+  </si>
+  <si>
+    <t>F10 é a taxa, f9 é o periodo,0 é o pagamento este valor não foi utilizado na fórmula, mas é o pagamento intermediário. f6 é o valor da duplicata está com o (-) na frente para não aparecer um valor negativo como resultado</t>
+  </si>
+  <si>
+    <t>e o tipo é quando a taxa de juros -pagamento sera aplicado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+  <numFmts count="4">
+    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -252,10 +272,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -275,25 +295,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -305,29 +319,56 @@
     <xf numFmtId="10" fontId="5" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -647,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,11 +737,11 @@
         <v>2</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="16" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="5"/>
@@ -709,158 +750,232 @@
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7">
+        <v>90000</v>
+      </c>
       <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7">
+        <v>3000</v>
+      </c>
       <c r="H6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7">
+        <v>10000</v>
+      </c>
     </row>
     <row r="7" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="9">
+        <v>10000</v>
+      </c>
       <c r="E7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="19"/>
+      <c r="F7" s="17">
+        <v>43819</v>
+      </c>
       <c r="H7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="19"/>
+      <c r="I7" s="17">
+        <v>43728</v>
+      </c>
     </row>
     <row r="8" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9">
+        <f>C6-C7</f>
+        <v>80000</v>
+      </c>
       <c r="E8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="17">
+        <v>43728</v>
+      </c>
       <c r="H8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="19"/>
+      <c r="I8" s="17">
+        <v>44094</v>
+      </c>
     </row>
     <row r="9" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="13">
+        <v>36</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="20"/>
+      <c r="F9" s="27">
+        <f>(F7-F8)/30</f>
+        <v>3.0333333333333332</v>
+      </c>
       <c r="H9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="20"/>
+      <c r="I9" s="18">
+        <f>(I8-I7)/30</f>
+        <v>12.2</v>
+      </c>
     </row>
     <row r="10" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="14">
+        <v>0.01</v>
+      </c>
       <c r="E10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="19">
+        <v>0.02</v>
+      </c>
       <c r="H10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="21"/>
+      <c r="I10" s="19">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="11" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="23">
+        <f>PMT(C10,C9,-C8,0,0)</f>
+        <v>2657.1447850280956</v>
+      </c>
       <c r="E11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="23"/>
+      <c r="F11" s="29">
+        <f>F6-F12</f>
+        <v>174.89842641592077</v>
+      </c>
       <c r="H11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="22"/>
+      <c r="I11" s="20">
+        <f>FV(I10,I9,0,-I6,0)</f>
+        <v>11290.697193038357</v>
+      </c>
     </row>
     <row r="12" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="22">
+        <f>C11*C9</f>
+        <v>95657.212261011446</v>
+      </c>
       <c r="E12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="22"/>
+      <c r="F12" s="28">
+        <f>PV(F10,F9,0,-F6,0)</f>
+        <v>2825.1015735840792</v>
+      </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="24">
+        <f>C12-C8</f>
+        <v>15657.212261011446</v>
+      </c>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="17"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E15" s="17"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="17"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="17"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="17"/>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E27" s="17"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E28" s="17"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E29" s="17"/>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="17"/>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="15"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>